<commit_message>
Added new Code for STO Project(Project redirection, Breadcrumb and Profile Matching)
</commit_message>
<xml_diff>
--- a/bin/com/qa/testdata/abcd.xlsx
+++ b/bin/com/qa/testdata/abcd.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="LTTS" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="30">
   <si>
     <t xml:space="preserve">Path</t>
   </si>
@@ -31,7 +32,10 @@
     <t xml:space="preserve">StatusMessage</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.hcltech.com/press-releases/life-sciences-and-healthcare/hcl-selected-blue-cross-and-blue-shield-association</t>
+    <t xml:space="preserve">200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.hcltech.com/press-releases/awards-recognitions/hcl-technologies-named-top-financial-services-technology-provid-0</t>
@@ -59,6 +63,48 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.hcltech.com/press-releases/americas/hcl-and-cforia-partner-improve-clients-accounts-receivable-portfolios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.lnttechservices.com/engineering-the-change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.lnttechservices.com/industry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.lnttechservices.com/industry/industrial-products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.lnttechservices.com/industry/medical-devices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.lnttechservices.com/industry/consumer-electronics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.lnttechservices.com/industry/plant-engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.lnttechservices.com/industry/media-entertainment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.lnttechservices.com/industry/oil-and-gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.lnttechservices.com/industry/semiconductors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.lnttechservices.com/industry/telecommunications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.lnttechservices.com/industry/transportation</t>
+  </si>
+  <si>
+    <t>StatusCode</t>
+  </si>
+  <si>
+    <t>StatusMessage</t>
   </si>
   <si>
     <t>200</t>
@@ -104,7 +150,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,6 +161,26 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00FF66"/>
         <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
       </patternFill>
     </fill>
   </fills>
@@ -159,7 +225,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -176,6 +242,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -255,15 +323,15 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="58.3163265306122" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" hidden="false" style="0" width="10.52734375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" hidden="false" style="0" width="13.5625" collapsed="true"/>
+    <col min="1" max="1" hidden="false" style="0" width="55.4795918367347" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="9.98979591836735" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="12.9591836734694" collapsed="true"/>
     <col min="4" max="1025" hidden="false" style="0" width="8.36734693877551" collapsed="true"/>
   </cols>
   <sheetData>
@@ -278,114 +346,112 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3"/>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" t="s">
-        <v>14</v>
+      <c r="B11" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -397,4 +463,165 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col min="1" max="1" hidden="false" style="0" width="33.6122448979592" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.52734375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.5625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s" s="4">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s" s="5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>